<commit_message>
update DE, fisherExact and GSEA
</commit_message>
<xml_diff>
--- a/doc/190125_scRNAseq_info.xlsx
+++ b/doc/190125_scRNAseq_info.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yah2014/Dropbox/Public/Olivier/Projects/scRNAseq-LorenzoBlood/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27458C5A-9FA9-CF4C-ACEF-91CCFC878E46}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27458C5A-9FA9-CF4C-ACEF-91CCFC878E46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42240" yWindow="1940" windowWidth="28020" windowHeight="16480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scRNA-seq" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,61 +35,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
+    <t>Sample.ID</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Submitter</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Tissue</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
     <t>tests</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Submitter</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Library</t>
-  </si>
-  <si>
-    <t>Sample.ID</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Conditions</t>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>Aitziber Buqué Martinez</t>
+  </si>
+  <si>
+    <t>Mus_musculus</t>
   </si>
   <si>
     <t>NSC</t>
   </si>
   <si>
+    <t>NAM</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
     <t>GSC827</t>
-  </si>
-  <si>
-    <t>Tissue</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>NAM</t>
-  </si>
-  <si>
-    <t>control</t>
-  </si>
-  <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>Aitziber Buqué Martinez</t>
-  </si>
-  <si>
-    <t>Mus_musculus</t>
   </si>
   <si>
     <t>test1</t>
@@ -91,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -320,87 +328,138 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="149">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
@@ -408,66 +467,15 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -808,116 +816,116 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="5">
         <v>43467</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="18">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5">
         <v>43467</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="18">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -930,7 +938,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="18">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -943,7 +951,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="18">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -956,7 +964,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="18">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -969,7 +977,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="18">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -982,7 +990,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="18">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -995,7 +1003,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="18">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1008,7 +1016,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="18">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1021,7 +1029,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="18">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1034,7 +1042,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="18">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1047,7 +1055,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="18">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1057,7 +1065,7 @@
       <c r="H14" s="6"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="18">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>

</xml_diff>